<commit_message>
docs: update data dicitionary and data modeling
</commit_message>
<xml_diff>
--- a/back-end/data-dictionary.xlsx
+++ b/back-end/data-dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\task-plus\back-end\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A7F0CA2-D2CC-4096-8366-6D92C4DFBF63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9643607A-EA1F-4E34-AB2C-E422DC5A2570}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" xr2:uid="{930CAEE1-5B1E-47D8-A4DE-5C9FFF5A2229}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Tabela</t>
   </si>
@@ -99,9 +99,6 @@
     <t>TIMESTAMP WITHOUT TIME ZONE</t>
   </si>
   <si>
-    <t>comment_id</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -112,13 +109,25 @@
   </si>
   <si>
     <t>Conteúdo do comentário.</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>user_name</t>
+  </si>
+  <si>
+    <t>Nome do usuário que cadastrou a task.</t>
+  </si>
+  <si>
+    <t>Data do comentário cadastrado.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +137,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -237,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -245,6 +262,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -254,9 +274,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D9E010-F8C1-4D33-8CF2-BED738885A80}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,11 +625,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -621,7 +642,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
@@ -636,7 +657,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
@@ -651,7 +672,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
@@ -666,17 +687,17 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -705,11 +726,11 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>25</v>
+      <c r="A9" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
@@ -718,44 +739,81 @@
         <v>6</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="12"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A9:A13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>